<commit_message>
Update admin, Staff, Doctor Frontend
</commit_message>
<xml_diff>
--- a/doc/SE1810_3/SWP391-Group3-Project Tracking.xlsx
+++ b/doc/SE1810_3/SWP391-Group3-Project Tracking.xlsx
@@ -14,14 +14,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="yqQduVPWLDocXZSfkT9rKrDsNz4jG23HhZvJdTh0+XA="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="3Y8zstZ14z0N+rBlzNGmMG5O4OTHXFMVnBBO/qUhibg="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="189">
   <si>
     <t>SWP391 - Group 1</t>
   </si>
@@ -571,25 +571,37 @@
     <t>Write all DAO classes to access data from database</t>
   </si>
   <si>
-    <t>Complete update table in UC-E-1-1, UC-E-1-2, UC-E-1-3</t>
-  </si>
-  <si>
-    <t>Complete update table in UC-E-2-1, UC-E-2-2, UC-E-2-3, UC-E-2-4</t>
-  </si>
-  <si>
-    <t>Complete update table in UC-E-3-1, UC-E-3-2, UC-E-3-3, UC-E-3-4</t>
-  </si>
-  <si>
-    <t>Complete update table in UC-E-4-1, UC-E-4-2, UC-E-4-3, UC-E-4-4, UC-E-4-5, UC-E-4-6, UC-E-4-7, UC-E-4-8</t>
-  </si>
-  <si>
-    <t>Complete update table in UC-E-5-1, UC-E-5-2, UC-E-5-3, UC-E-5-4, UC-E-5-5</t>
-  </si>
-  <si>
-    <t>Complete update table in UC-E-6-1, UC-E-6-2, UC-E-6-3</t>
-  </si>
-  <si>
-    <t>Complete update table in UC-E-7-1, UC-E-7-2, UC-E-7-3, UC-E-7-4</t>
+    <t>Complete update table in UC-E-1-1, UC-E-1-2, UC-E-1-3
+Complete update table in UC-E-2-1, UC-E-2-2, UC-E-2-3, UC-E-2-4
+Complete update table in UC-E-3-1, UC-E-3-2, UC-E-3-3, UC-E-3-4
+Complete update table in UC-E-4-1, UC-E-4-2, UC-E-4-3, UC-E-4-4, UC-E-4-5, UC-E-4-6, UC-E-4-7, UC-E-4-8
+Complete update table in UC-E-5-1, UC-E-5-2, UC-E-5-3, UC-E-5-4, UC-E-5-5
+Complete update table in UC-E-6-1, UC-E-6-2, UC-E-6-3
+Complete update table in UC-E-7-1, UC-E-7-2, UC-E-7-3, UC-E-7-4</t>
+  </si>
+  <si>
+    <t>Project Development</t>
+  </si>
+  <si>
+    <t>Code UC-E-1-1, UC-E-1-2, UC-E-1-3</t>
+  </si>
+  <si>
+    <t>Code UC-E-2-1, UC-E-2-2, UC-E-2-3, UC-E-2-4</t>
+  </si>
+  <si>
+    <t>Code UC-E-3-1, UC-E-3-2, UC-E-3-3, UC-E-3-4</t>
+  </si>
+  <si>
+    <t>Code  UC-E-4-1, UC-E-4-2, UC-E-4-3, UC-E-4-4, UC-E-4-5, UC-E-4-6, UC-E-4-7, UC-E-4-8</t>
+  </si>
+  <si>
+    <t>Code UC-E-5-1, UC-E-5-2, UC-E-5-3, UC-E-5-4, UC-E-5-5</t>
+  </si>
+  <si>
+    <t>Code UC-E-6-1, UC-E-6-2, UC-E-6-3</t>
+  </si>
+  <si>
+    <t>Code UC-E-7-1, UC-E-7-2, UC-E-7-3, UC-E-7-4</t>
   </si>
   <si>
     <t>Edit video User manual</t>
@@ -667,7 +679,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -692,8 +704,20 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB3CEFA"/>
+        <bgColor rgb="FFB3CEFA"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border/>
     <border>
       <left style="thin">
@@ -832,11 +856,22 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="72">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -967,6 +1002,66 @@
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="16" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="16" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="16" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="16" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="16" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="17" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="14" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="6" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="16" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="15" fillId="6" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="16" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1040,7 +1135,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="7">
+  <tableStyles count="6">
     <tableStyle count="3" pivot="0" name="Infomation-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -1062,11 +1157,6 @@
       <tableStyleElement dxfId="6" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="Iteration2-style">
-      <tableStyleElement dxfId="4" type="headerRow"/>
-      <tableStyleElement dxfId="5" type="firstRowStripe"/>
-      <tableStyleElement dxfId="6" type="secondRowStripe"/>
-    </tableStyle>
-    <tableStyle count="3" pivot="0" name="Iteration3-style">
       <tableStyleElement dxfId="4" type="headerRow"/>
       <tableStyleElement dxfId="5" type="firstRowStripe"/>
       <tableStyleElement dxfId="6" type="secondRowStripe"/>
@@ -1186,24 +1276,6 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A5:J16" displayName="Table_6" name="Table_6" id="6">
-  <tableColumns count="10">
-    <tableColumn name="#" id="1"/>
-    <tableColumn name="Title" id="2"/>
-    <tableColumn name="Description" id="3"/>
-    <tableColumn name="Actor" id="4"/>
-    <tableColumn name="Assignee" id="5"/>
-    <tableColumn name="Status" id="6"/>
-    <tableColumn name="Priority" id="7"/>
-    <tableColumn name="SRS" id="8"/>
-    <tableColumn name="SDS" id="9"/>
-    <tableColumn name="Note" id="10"/>
-  </tableColumns>
-  <tableStyleInfo name="Iteration3-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A5:J16" displayName="Table_7" name="Table_7" id="7">
   <tableColumns count="10">
     <tableColumn name="#" id="1"/>
     <tableColumn name="Title" id="2"/>
@@ -12429,7 +12501,7 @@
     <col customWidth="1" min="3" max="3" width="89.5"/>
     <col customWidth="1" min="4" max="4" width="14.38"/>
     <col customWidth="1" min="5" max="5" width="25.13"/>
-    <col customWidth="1" min="6" max="6" width="9.88"/>
+    <col customWidth="1" min="6" max="6" width="13.38"/>
     <col customWidth="1" min="7" max="10" width="18.88"/>
     <col customWidth="1" min="11" max="11" width="2.63"/>
   </cols>
@@ -12469,310 +12541,315 @@
       <c r="A4" s="25"/>
     </row>
     <row r="5" ht="22.5" customHeight="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="50" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" ht="30.0" customHeight="1">
-      <c r="A6" s="29">
+    <row r="6">
+      <c r="A6" s="52">
         <v>1.0</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32" t="s">
+      <c r="D6" s="54"/>
+      <c r="E6" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="55">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="54"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+    </row>
+    <row r="7" ht="30.0" customHeight="1">
+      <c r="A7" s="57">
+        <v>2.0</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+    </row>
+    <row r="8" ht="30.0" customHeight="1">
+      <c r="A8" s="52">
+        <v>3.0</v>
+      </c>
+      <c r="B8" s="63"/>
+      <c r="C8" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="54"/>
+      <c r="E8" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="G6" s="32">
+      <c r="F8" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="55">
         <v>1.0</v>
       </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-    </row>
-    <row r="7" ht="30.0" customHeight="1">
-      <c r="A7" s="29">
+      <c r="H8" s="54"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+    </row>
+    <row r="9" ht="30.0" customHeight="1">
+      <c r="A9" s="57">
+        <v>4.0</v>
+      </c>
+      <c r="B9" s="64"/>
+      <c r="C9" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" s="60"/>
+      <c r="E9" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="H9" s="60"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+    </row>
+    <row r="10" ht="30.0" customHeight="1">
+      <c r="A10" s="52">
+        <v>5.0</v>
+      </c>
+      <c r="B10" s="63"/>
+      <c r="C10" s="53" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="54"/>
+      <c r="E10" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="55">
+        <v>1.0</v>
+      </c>
+      <c r="H10" s="54"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+    </row>
+    <row r="11" ht="30.0" customHeight="1">
+      <c r="A11" s="57">
+        <v>6.0</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="65"/>
+      <c r="E11" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="H11" s="60"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+    </row>
+    <row r="12" ht="30.0" customHeight="1">
+      <c r="A12" s="52">
+        <v>7.0</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="53" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="55">
+        <v>1.0</v>
+      </c>
+      <c r="H12" s="54"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+    </row>
+    <row r="13" ht="30.0" customHeight="1">
+      <c r="A13" s="57">
+        <v>8.0</v>
+      </c>
+      <c r="B13" s="67"/>
+      <c r="C13" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="D13" s="65"/>
+      <c r="E13" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="H13" s="60"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+    </row>
+    <row r="14" ht="30.0" customHeight="1">
+      <c r="A14" s="52">
+        <v>9.0</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="66"/>
+      <c r="E14" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="55">
+        <v>3.0</v>
+      </c>
+      <c r="H14" s="54"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+    </row>
+    <row r="15" ht="30.0" customHeight="1">
+      <c r="A15" s="57">
+        <v>10.0</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="61">
         <v>2.0</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="H15" s="60"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
+    </row>
+    <row r="16" ht="30.0" customHeight="1">
+      <c r="A16" s="52">
+        <v>11.0</v>
+      </c>
+      <c r="B16" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="71" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="55">
+        <v>3.0</v>
+      </c>
+      <c r="H16" s="54"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+    </row>
+    <row r="17" ht="30.0" customHeight="1">
+      <c r="A17" s="57">
+        <v>12.0</v>
+      </c>
+      <c r="B17" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="G7" s="32">
+      <c r="C17" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="65"/>
+      <c r="E17" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="61">
         <v>1.0</v>
       </c>
-      <c r="H7" s="31"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-    </row>
-    <row r="8" ht="30.0" customHeight="1">
-      <c r="A8" s="29">
-        <v>3.0</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="G8" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-    </row>
-    <row r="9" ht="30.0" customHeight="1">
-      <c r="A9" s="29">
-        <v>4.0</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>182</v>
-      </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="G9" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="H9" s="31"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" ht="30.0" customHeight="1">
-      <c r="A10" s="29">
-        <v>5.0</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="G10" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" ht="30.0" customHeight="1">
-      <c r="A11" s="29">
-        <v>6.0</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="G11" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="H11" s="31"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" ht="30.0" customHeight="1">
-      <c r="A12" s="29">
-        <v>7.0</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="G12" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" ht="30.0" customHeight="1">
-      <c r="A13" s="29">
-        <v>8.0</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="G13" s="32">
-        <v>3.0</v>
-      </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-    </row>
-    <row r="14" ht="30.0" customHeight="1">
-      <c r="A14" s="29">
-        <v>9.0</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="G14" s="32">
-        <v>2.0</v>
-      </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-    </row>
-    <row r="15" ht="30.0" customHeight="1">
-      <c r="A15" s="29">
-        <v>10.0</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="G15" s="32">
-        <v>3.0</v>
-      </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-    </row>
-    <row r="16" ht="30.0" customHeight="1">
-      <c r="A16" s="29">
-        <v>11.0</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="G16" s="32">
-        <v>1.0</v>
-      </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-    </row>
-    <row r="17" ht="15.0" customHeight="1">
-      <c r="A17" s="25"/>
-      <c r="K17" s="25"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+    </row>
+    <row r="18" ht="15.0" customHeight="1">
+      <c r="A18" s="25"/>
+      <c r="K18" s="25"/>
+    </row>
     <row r="19" ht="15.75" customHeight="1"/>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -13720,15 +13797,17 @@
     <row r="963" ht="15.75" customHeight="1"/>
     <row r="964" ht="15.75" customHeight="1"/>
     <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J3"/>
-    <mergeCell ref="K2:K16"/>
+    <mergeCell ref="K2:K17"/>
     <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="B7:B13"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:A16">
+  <conditionalFormatting sqref="A6:A17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -13741,13 +13820,13 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E6:E16">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E6:E17">
       <formula1>Infomation!$C$9:$C$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F6:F16">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F6:F17">
       <formula1>"Backlog,In progress,Ready,In testing,Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G6:G16">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G6:G17">
       <formula1>"1,2,3"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13755,9 +13834,6 @@
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -14080,7 +14156,7 @@
         <v>145</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="32" t="s">

</xml_diff>